<commit_message>
Add some documents for our source
</commit_message>
<xml_diff>
--- a/医疗健康事业部KPI/2018年第二季度KPI/2018年第2季度员工个人绩效考核目标-王德文.xlsx
+++ b/医疗健康事业部KPI/2018年第二季度KPI/2018年第2季度员工个人绩效考核目标-王德文.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devin.wong/Documents/Work/楚天云/医疗健康事业部/2018年一级部门组织绩效考核目标- 医疗健康事业部/二季度考核目标/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devin.wong/Documents/Repository/medical_technology_group/医疗健康事业部KPI/2018年第二季度KPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5259205A-75DF-614F-AEB5-BC420BF168C8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B8170608-E096-784D-B1E8-D3D8F1D28DC6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,14 +197,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>1、支撑智慧健康产业公司商业计划书完成，形成董事会决议；10分
-2、带领团队入场武汉市卫计委，配合卫计委、管理并执行卫计委安排的工作。15分
-3、带领团队进行健康武汉APP推广支撑与开发管理；15分
-4、带领团队配合专家团队完成健康武汉项目系统规格造价；15分
-5、启动商保服务、云药房、影像云的厂商技术对接，形成实质性改造方案与实施策略；115分</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>1、协助运营对接合作厂商，支撑运营点的技术方案输出、对接；10分
 2、带领团队协助卫计委完成“健康武汉”APP、互联网入口在楚天云的部署、运行维护；并支撑运营；10分
 3、配合公司公共技术部需求调研；10分</t>
@@ -220,6 +212,14 @@
   </si>
   <si>
     <t>湖北省楚天云有限公司2018年第2季度个人绩效考核</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、支撑智慧健康产业公司商业计划书完成，形成董事会决议；10分
+2、带领团队入场武汉市卫计委，配合卫计委、管理并执行卫计委安排的工作。15分
+3、带领团队进行健康武汉APP推广支撑与开发管理；15分
+4、带领团队配合专家团队完成健康武汉项目系统规格造价；15分
+5、启动商保服务、云药房、影像云的厂商技术对接，形成实质性改造方案与实施策略；15分</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -826,7 +826,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -843,7 +843,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -923,7 +923,7 @@
         <v>0.7</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>11</v>
@@ -942,7 +942,7 @@
         <v>0.3</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>3</v>
@@ -957,7 +957,7 @@
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="9" t="s">

</xml_diff>